<commit_message>
Clean repo: removed unnecessary files
</commit_message>
<xml_diff>
--- a/src/main/resources/FeatureFiles/FirefoxTestFileStable.xlsx
+++ b/src/main/resources/FeatureFiles/FirefoxTestFileStable.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="74">
   <si>
     <t>Test Case Id</t>
   </si>
@@ -48,106 +48,196 @@
     <t>sumit.tomar@algoworks.com</t>
   </si>
   <si>
+    <t>triggerLazyLoadAndClick</t>
+  </si>
+  <si>
+    <t>ContactPage_TextBox_FirstName</t>
+  </si>
+  <si>
+    <t>ContactPage_TextBox_LastName</t>
+  </si>
+  <si>
+    <t>ContactPage_TextBox_PhoneNumber</t>
+  </si>
+  <si>
+    <t>selectValueFromDropDown</t>
+  </si>
+  <si>
+    <t>ContactPage_DropDown_Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>ContactPage_DropDown_JobTitle</t>
+  </si>
+  <si>
+    <t>ContactPage_DropDown_ReasonForInquiry</t>
+  </si>
+  <si>
+    <t>9911223344</t>
+  </si>
+  <si>
+    <t>ContactPage_TextBox_CompanyName</t>
+  </si>
+  <si>
+    <t>Algoworks</t>
+  </si>
+  <si>
+    <t>ContactPage_TextBox_CommentBox</t>
+  </si>
+  <si>
+    <t>Test case 2</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>ContactPage_Button_ContactUs</t>
+  </si>
+  <si>
+    <t>ContactPage_CheckMark_SuccessfullConfirmation</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>Support Request</t>
+  </si>
+  <si>
+    <t>Analyst / Press</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>textBoxMustHaveValue</t>
+  </si>
+  <si>
+    <t>Sumit</t>
+  </si>
+  <si>
+    <t>To-mar</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>All fields are valid</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>gotoUrl</t>
+  </si>
+  <si>
+    <t>ContactPage_BrandLogo_ImageLink</t>
+  </si>
+  <si>
+    <t>waitForPageToRender</t>
+  </si>
+  <si>
+    <t>beforeEach</t>
+  </si>
+  <si>
+    <t>afterEach</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>sumit.tomar#algoworks.com</t>
+  </si>
+  <si>
+    <t>pressKey</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>ContactPage_ErrorMessage_InvalidEmail_TextBox_Email</t>
+  </si>
+  <si>
+    <t>elementMustHaveText</t>
+  </si>
+  <si>
+    <t>Must be a valid email address.</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>S123456</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>ContactPage_ErrorMessage_InvalidFirstName_TextBox_FirstName</t>
+  </si>
+  <si>
+    <t>Please enter a valid name.</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>-?/!@</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>ContactPage_ErrorMessage_InvalidLastName_TextBox_LastName</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>tomar</t>
+  </si>
+  <si>
+    <t>99112</t>
+  </si>
+  <si>
+    <t>ContactPage_ErrorMessage_InvalidPhoneNumber_TextBox_PhoneNumber</t>
+  </si>
+  <si>
+    <t>Please enter a valid phone number.</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>9991127890</t>
+  </si>
+  <si>
+    <t>ContactPage_ErrorMessage_EmptyField_TextBox_Company</t>
+  </si>
+  <si>
+    <t>This field is required.</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>ContactPage_ErrorMessage_EmptyField_Dropdown_JobTitle</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>ContactPage_ErrorMessage_EmptyField_Dropdown_Country</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>ContactPage_ErrorMessage_EmptyField_Dropdown_ReasonForInquiry</t>
+  </si>
+  <si>
     <t>openBrowser</t>
-  </si>
-  <si>
-    <t>triggerLazyLoadAndClick</t>
-  </si>
-  <si>
-    <t>ContactPage_TextBox_FirstName</t>
-  </si>
-  <si>
-    <t>ContactPage_TextBox_LastName</t>
-  </si>
-  <si>
-    <t>ContactPage_TextBox_PhoneNumber</t>
-  </si>
-  <si>
-    <t>selectValueFromDropDown</t>
-  </si>
-  <si>
-    <t>ContactPage_DropDown_Country</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>ContactPage_DropDown_JobTitle</t>
-  </si>
-  <si>
-    <t>ContactPage_DropDown_ReasonForInquiry</t>
-  </si>
-  <si>
-    <t>9911223344</t>
-  </si>
-  <si>
-    <t>ContactPage_TextBox_CompanyName</t>
-  </si>
-  <si>
-    <t>Algoworks</t>
-  </si>
-  <si>
-    <t>ContactPage_TextBox_CommentBox</t>
-  </si>
-  <si>
-    <t>Test case 2</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>ContactPage_Button_ContactUs</t>
-  </si>
-  <si>
-    <t>ContactPage_CheckMark_SuccessfullConfirmation</t>
-  </si>
-  <si>
-    <t>TC001</t>
-  </si>
-  <si>
-    <t>Support Request</t>
-  </si>
-  <si>
-    <t>Analyst / Press</t>
-  </si>
-  <si>
-    <t>closeBrowser</t>
-  </si>
-  <si>
-    <t>textBoxMustHaveValue</t>
-  </si>
-  <si>
-    <t>Sumit</t>
-  </si>
-  <si>
-    <t>To-mar</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>All fields are valid</t>
-  </si>
-  <si>
-    <t>TC002</t>
-  </si>
-  <si>
-    <t>gotoUrl</t>
-  </si>
-  <si>
-    <t>ContactPage_BrandLogo_ImageLink</t>
-  </si>
-  <si>
-    <t>waitForPageToRender</t>
-  </si>
-  <si>
-    <t>beforeEach</t>
-  </si>
-  <si>
-    <t>afterEach</t>
-  </si>
-  <si>
-    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -214,8 +304,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -518,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,26 +639,26 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
@@ -577,12 +669,12 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -590,15 +682,12 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -612,12 +701,12 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -626,21 +715,21 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -648,21 +737,21 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -670,54 +759,54 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -725,10 +814,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -736,18 +825,18 @@
         <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -755,12 +844,12 @@
         <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>7</v>
@@ -769,128 +858,114 @@
         <v>8</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>32</v>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="2" t="s">
-        <v>15</v>
+      <c r="B33" t="s">
+        <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="2" t="s">
-        <v>7</v>
+      <c r="B35" t="s">
+        <v>31</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -898,40 +973,1111 @@
         <v>7</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="2" t="s">
-        <v>25</v>
+      <c r="B37" t="s">
+        <v>31</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>31</v>
+      <c r="C44" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B55" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B56" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B57" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B60" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B62" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B73" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B74" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B75" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B77" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B78" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B79" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>31</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B83" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>31</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B85" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B86" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B87" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B88" t="s">
+        <v>31</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B89" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B91" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B92" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B93" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B95" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B98" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B99" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B101" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B102" t="s">
+        <v>31</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B103" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B104" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B105" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B106" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B107" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B108" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B109" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B111" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B114" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B115" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B116" t="s">
+        <v>31</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B117" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D117" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B118" t="s">
+        <v>31</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B119" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B120" t="s">
+        <v>31</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B121" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B122" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B123" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B124" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B125" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B126" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B127" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A129" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B130" t="s">
+        <v>31</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B131" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B132" t="s">
+        <v>31</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B133" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B134" t="s">
+        <v>31</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B135" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B136" t="s">
+        <v>31</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B137" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B138" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B139" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B140" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B141" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B142" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B143" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D143" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D51" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>